<commit_message>
update for fa 2018
</commit_message>
<xml_diff>
--- a/_includes/course-schedule.xlsx
+++ b/_includes/course-schedule.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t xml:space="preserve">Last day to drop a class without a grade </t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>P266.pdf</t>
+  </si>
+  <si>
+    <t>Rahel, F. J. 2016. Changing Philosophies of Fisheries Management as Illustrated by the History of Fishing Regulations in Wyoming. Fisheries 41:38-48.</t>
+  </si>
+  <si>
+    <t>R189.pdf</t>
+  </si>
+  <si>
+    <t>Whelan, G. 2004. A historical perspective on the use of propogated fish in fisheries management: Michigan's 130-year experience. American Fisheries Society Symposium 44:307-315.</t>
+  </si>
+  <si>
+    <t>W205.pdf</t>
   </si>
 </sst>
 </file>
@@ -629,10 +641,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +678,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D11" si="0">CONCATENATE(B2," [pdf](pdfs/",C2,")")</f>
+        <f t="shared" ref="D2:D13" si="0">CONCATENATE(B2," [pdf](pdfs/",C2,")")</f>
         <v>Bennett, D. H., E. L. Hampton, and R. T. Lackey. 1978. Current and future fisheries management goals: Implications for future management. Fisheries 3:10-14. [pdf](pdfs/B269.pdf)</v>
       </c>
     </row>
@@ -730,7 +742,7 @@
         <v>Nielsen, L. A. 1995. The practical uses of fisheries history. Fisheries 20:16-18. [pdf](pdfs/N51.pdf)</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -760,7 +772,7 @@
         <v>Pauly, D. 2001. Fisheries Management. John Wiley &amp; Sons, Ltd. [pdf](pdfs/P178.pdf)</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -801,6 +813,36 @@
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Pascoe, S., K. Brooks, T. Cannard, C. M. Dichmont, E. Jebreen, J. Schirmer, and L. Triantafillos. 2014. Social objectives of fisheries management: What are managers' priorities? Ocean and Coastal Management 98:1-10. [pdf](pdfs/P266.pdf)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Rahel, F. J. 2016. Changing Philosophies of Fisheries Management as Illustrated by the History of Fishing Regulations in Wyoming. Fisheries 41:38-48. [pdf](pdfs/R189.pdf)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Whelan, G. 2004. A historical perspective on the use of propogated fish in fisheries management: Michigan's 130-year experience. American Fisheries Society Symposium 44:307-315. [pdf](pdfs/W205.pdf)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>